<commit_message>
API-Automated_testing V1.1: Added comments for all classes and methods
</commit_message>
<xml_diff>
--- a/tests/data/test_data.xlsx
+++ b/tests/data/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharmProject\api-automated-testing\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D68D870-4A61-4632-BD94-7A47E4D0A74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26B65F8-1D0D-4574-960C-D393B1F64A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1245" yWindow="3225" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterData" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -588,32 +588,49 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
+    <col min="2" max="2" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>